<commit_message>
added v1 nozzle CAD and updated nozzle design equations doc
</commit_message>
<xml_diff>
--- a/Nozzle/Converse Engine v1.xlsx
+++ b/Nozzle/Converse Engine v1.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Nozzle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C619788-F87A-494E-AFE1-6FEBCC715D8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93A7A51-28FF-DE43-A1A7-C1F15B048FF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16540" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16520" activeTab="1" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Description" sheetId="1" r:id="rId1"/>
+    <sheet name="Stats" sheetId="2" r:id="rId1"/>
+    <sheet name="Description" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Nozzle</t>
   </si>
@@ -58,13 +59,76 @@
   </si>
   <si>
     <t>Nozzle Throat Gas Temperature (t)</t>
+  </si>
+  <si>
+    <t>Propellant Flow Rate</t>
+  </si>
+  <si>
+    <t>Thrust / Impulse</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Calculations</t>
+  </si>
+  <si>
+    <t>Aimed Thrust Capacity</t>
+  </si>
+  <si>
+    <t>lbf</t>
+  </si>
+  <si>
+    <t>Propellants:</t>
+  </si>
+  <si>
+    <t>Ethanol</t>
+  </si>
+  <si>
+    <t>"+"</t>
+  </si>
+  <si>
+    <t>Liquid Oxygen</t>
+  </si>
+  <si>
+    <t>Impulse</t>
+  </si>
+  <si>
+    <t>Combustion Temperature</t>
+  </si>
+  <si>
+    <t>Chamber Pressure</t>
+  </si>
+  <si>
+    <t>Oxidizer Flow Rate</t>
+  </si>
+  <si>
+    <t>Fuel Flow Rate</t>
+  </si>
+  <si>
+    <t>Throat Temperature</t>
+  </si>
+  <si>
+    <t>Chamber Temperature</t>
+  </si>
+  <si>
+    <t>Throat Pressure</t>
+  </si>
+  <si>
+    <t>Throat Diameter</t>
+  </si>
+  <si>
+    <t>Propellant Flow Rate - Fuel Flow Rate</t>
+  </si>
+  <si>
+    <t>(Propellant Flow Rate / Mixture Ratio) + 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -82,6 +146,14 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,17 +176,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -136,16 +209,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>25399</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>139699</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>26653</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>140953</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -168,7 +241,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9309100" y="431799"/>
+          <a:off x="14744700" y="139699"/>
           <a:ext cx="4940300" cy="3201654"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -477,11 +550,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0A97E6-915A-D143-A6DF-A3F09B431841}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1">
+        <v>23000</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D475DE-CC2C-7C4E-9119-639F39D169A8}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -489,97 +621,193 @@
     <col min="1" max="1" width="35.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="K2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C5" s="1" t="s">
+      <c r="E4" s="1"/>
+      <c r="K4" s="4">
+        <v>65</v>
+      </c>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C6" s="1" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C7" s="1" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="9" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="9" spans="1:12" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="11" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="K9" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="11" spans="1:12" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="13" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="K11" s="4">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="13" spans="1:12" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="16">
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K11:L11"/>
     <mergeCell ref="C7:H7"/>
     <mergeCell ref="C9:H9"/>
     <mergeCell ref="C11:H11"/>

</xml_diff>

<commit_message>
update to documentation and minimal file-folder repo change
</commit_message>
<xml_diff>
--- a/Nozzle/Converse Engine v1.xlsx
+++ b/Nozzle/Converse Engine v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Nozzle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93A7A51-28FF-DE43-A1A7-C1F15B048FF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB621FC-30A5-0F4B-91DC-0BBBA9967F49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16520" activeTab="1" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Stats" sheetId="2" r:id="rId1"/>
     <sheet name="Description" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
   <si>
     <t>Nozzle</t>
   </si>
@@ -46,24 +46,12 @@
     <t>R = 1545.32 / 24 = 64.28 ft-lb</t>
   </si>
   <si>
-    <t>Gamma (Ratio of Specific Heats)</t>
-  </si>
-  <si>
     <t>Gamma = 1.2</t>
   </si>
   <si>
-    <t>Eaths Gravitation (Gc)</t>
-  </si>
-  <si>
     <t>32.2 ft/sec^2</t>
   </si>
   <si>
-    <t>Nozzle Throat Gas Temperature (t)</t>
-  </si>
-  <si>
-    <t>Propellant Flow Rate</t>
-  </si>
-  <si>
     <t>Thrust / Impulse</t>
   </si>
   <si>
@@ -100,35 +88,113 @@
     <t>Chamber Pressure</t>
   </si>
   <si>
-    <t>Oxidizer Flow Rate</t>
-  </si>
-  <si>
-    <t>Fuel Flow Rate</t>
-  </si>
-  <si>
-    <t>Throat Temperature</t>
-  </si>
-  <si>
-    <t>Chamber Temperature</t>
-  </si>
-  <si>
-    <t>Throat Pressure</t>
-  </si>
-  <si>
-    <t>Throat Diameter</t>
-  </si>
-  <si>
     <t>Propellant Flow Rate - Fuel Flow Rate</t>
   </si>
   <si>
     <t>(Propellant Flow Rate / Mixture Ratio) + 1</t>
+  </si>
+  <si>
+    <t>Combustion Temperature + 460</t>
+  </si>
+  <si>
+    <t>0.909 * Chamber Temperature</t>
+  </si>
+  <si>
+    <t>0.564 * Chamber Pressure</t>
+  </si>
+  <si>
+    <t>SQRT(4 * Throat Aea / PI)</t>
+  </si>
+  <si>
+    <t>Propellant Flow Rate (wt)</t>
+  </si>
+  <si>
+    <t>Fuel Flow Rate (wf)</t>
+  </si>
+  <si>
+    <t>Oxidizer Flow Rate (wo)</t>
+  </si>
+  <si>
+    <t>Chamber Temperature (Tc)</t>
+  </si>
+  <si>
+    <t>Throat Temperature (Tt)</t>
+  </si>
+  <si>
+    <t>Throat Pressure (Pt)</t>
+  </si>
+  <si>
+    <t>Throat Diameter (Dt)</t>
+  </si>
+  <si>
+    <t>Throat Area (At)</t>
+  </si>
+  <si>
+    <t>(wt/ Pt) * SQRT((R * Tt) / (y * g)</t>
+  </si>
+  <si>
+    <t>Gamma (Ratio of Specific Heats)(y)</t>
+  </si>
+  <si>
+    <t>Earths Gravitation (g)</t>
+  </si>
+  <si>
+    <t>Exit Area (Ae)</t>
+  </si>
+  <si>
+    <t>Exit Diameter (De)</t>
+  </si>
+  <si>
+    <t>Nozzle Length (Lnozzle)</t>
+  </si>
+  <si>
+    <t>Convergent Length (Lconvergent)</t>
+  </si>
+  <si>
+    <t>Divergent Length (Ldivergent)</t>
+  </si>
+  <si>
+    <t>Chamber Volume (Vc)</t>
+  </si>
+  <si>
+    <t>Chamber Diameter (Dc)</t>
+  </si>
+  <si>
+    <t>3.65 * Throat Area</t>
+  </si>
+  <si>
+    <t>SQRT( 4 * Exit Area / Pi)</t>
+  </si>
+  <si>
+    <t>Covergent Length + Divergrnt Length</t>
+  </si>
+  <si>
+    <t>Chamber Area</t>
+  </si>
+  <si>
+    <t>Chamber Length</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>in^3</t>
+  </si>
+  <si>
+    <t>(Dt / 2) * SIN(RADIANS(a - 90 + 180)) / SIN(RADIANS(a)</t>
+  </si>
+  <si>
+    <t>(De / 2) * SIN(Nozzle Angles - 90 + 180) / SIN(Nozzle Angles)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -155,6 +221,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -176,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -184,10 +258,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -218,7 +298,7 @@
       <xdr:col>21</xdr:col>
       <xdr:colOff>482600</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>140953</xdr:rowOff>
+      <xdr:rowOff>179053</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -554,7 +634,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -564,43 +644,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>15</v>
+      <c r="A1" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="B1">
         <v>23000</v>
       </c>
       <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -610,10 +690,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D475DE-CC2C-7C4E-9119-639F39D169A8}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -622,24 +702,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="E2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="K2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="4"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="E2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="K2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="8"/>
     </row>
     <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -650,131 +730,149 @@
         <v>3</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="K4" s="4">
+      <c r="K4" s="6">
         <v>65</v>
       </c>
-      <c r="L4" s="4"/>
+      <c r="L4" s="6"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="9" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="K9" s="4">
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="K9" s="6">
         <v>1.2</v>
       </c>
-      <c r="L9" s="4"/>
+      <c r="L9" s="6"/>
     </row>
     <row r="11" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="K11" s="6">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="L11" s="6"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="K11" s="4">
-        <v>32.200000000000003</v>
-      </c>
-      <c r="L11" s="4"/>
-    </row>
-    <row r="13" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C21" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -782,28 +880,182 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>47</v>
+      </c>
+      <c r="I43" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="I45" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="E2:F2"/>
+  <mergeCells count="26">
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="C41:H41"/>
+    <mergeCell ref="C29:H29"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="C35:H35"/>
+    <mergeCell ref="C37:H37"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="C27:H27"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="K9:L9"/>
@@ -811,10 +1063,14 @@
     <mergeCell ref="C7:H7"/>
     <mergeCell ref="C9:H9"/>
     <mergeCell ref="C11:H11"/>
-    <mergeCell ref="C13:H13"/>
     <mergeCell ref="A1:C2"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C19:H19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>